<commit_message>
modified input to remove bad chars
</commit_message>
<xml_diff>
--- a/src/iNaturalist/data/11_10_18/2018_iNaturalist.xlsx
+++ b/src/iNaturalist/data/11_10_18/2018_iNaturalist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mccallm/Documents/GitHub/Pollinator_health/src/iNaturalist/data/10_26_18/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\localadmin\Desktop\iNat Python Script\Pollinator_health\src\iNaturalist\data\11_10_18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA25FBFB-FFD5-1A44-B43B-DCDC89E2903C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14640" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="observations-34528" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2812,7 +2811,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3163,25 +3162,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
+    <sheetView topLeftCell="A329" workbookViewId="0">
       <selection activeCell="B355" sqref="B355"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="16" max="16" width="33.1640625" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" customWidth="1"/>
-    <col min="18" max="18" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="6" max="6" width="19.625" customWidth="1"/>
+    <col min="16" max="16" width="33.125" customWidth="1"/>
+    <col min="17" max="17" width="19.875" customWidth="1"/>
+    <col min="18" max="18" width="29.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>493</v>
       </c>
@@ -3237,7 +3236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>14141175</v>
       </c>
@@ -3281,7 +3280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14141890</v>
       </c>
@@ -3325,7 +3324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14142248</v>
       </c>
@@ -3369,7 +3368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14142945</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14146448</v>
       </c>
@@ -3457,7 +3456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14147216</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14148296</v>
       </c>
@@ -3545,7 +3544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14149346</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>14169493</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>14169514</v>
       </c>
@@ -3677,7 +3676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>14170343</v>
       </c>
@@ -3721,7 +3720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14171054</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14179282</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14180498</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14204442</v>
       </c>
@@ -3897,7 +3896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14204855</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14205110</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14205498</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14205718</v>
       </c>
@@ -4070,7 +4069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14207628</v>
       </c>
@@ -4114,7 +4113,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14250234</v>
       </c>
@@ -4158,7 +4157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14250242</v>
       </c>
@@ -4202,7 +4201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14269245</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>14275191</v>
       </c>
@@ -4290,7 +4289,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14276963</v>
       </c>
@@ -4334,7 +4333,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>14277230</v>
       </c>
@@ -4378,7 +4377,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>14277981</v>
       </c>
@@ -4422,7 +4421,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14280225</v>
       </c>
@@ -4466,7 +4465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14291524</v>
       </c>
@@ -4510,7 +4509,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14291650</v>
       </c>
@@ -4554,7 +4553,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14294284</v>
       </c>
@@ -4598,7 +4597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>14294501</v>
       </c>
@@ -4642,7 +4641,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14300011</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>14300103</v>
       </c>
@@ -4730,7 +4729,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>14300186</v>
       </c>
@@ -4774,7 +4773,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>14301558</v>
       </c>
@@ -4818,7 +4817,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>14301620</v>
       </c>
@@ -4862,7 +4861,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>14301705</v>
       </c>
@@ -4906,7 +4905,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>14356673</v>
       </c>
@@ -4947,7 +4946,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>14357323</v>
       </c>
@@ -4988,7 +4987,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14367077</v>
       </c>
@@ -5032,7 +5031,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>14422375</v>
       </c>
@@ -5076,7 +5075,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>14422388</v>
       </c>
@@ -5120,7 +5119,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>14452279</v>
       </c>
@@ -5164,7 +5163,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14453600</v>
       </c>
@@ -5208,7 +5207,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14453873</v>
       </c>
@@ -5252,7 +5251,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>14454639</v>
       </c>
@@ -5296,7 +5295,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>14463592</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>14495551</v>
       </c>
@@ -5384,7 +5383,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>14509502</v>
       </c>
@@ -5428,7 +5427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>14509509</v>
       </c>
@@ -5472,7 +5471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>14509515</v>
       </c>
@@ -5516,7 +5515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>14509521</v>
       </c>
@@ -5560,7 +5559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>14515926</v>
       </c>
@@ -5604,7 +5603,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>14526838</v>
       </c>
@@ -5645,7 +5644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>14548675</v>
       </c>
@@ -5686,7 +5685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>14548778</v>
       </c>
@@ -5730,7 +5729,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>14548859</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>14554250</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>14581298</v>
       </c>
@@ -5859,7 +5858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>14587173</v>
       </c>
@@ -5903,7 +5902,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14596877</v>
       </c>
@@ -5947,7 +5946,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>14596902</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>14596911</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>14598280</v>
       </c>
@@ -6079,7 +6078,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>14598328</v>
       </c>
@@ -6123,7 +6122,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>14624235</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>14627591</v>
       </c>
@@ -6211,7 +6210,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>14653273</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>14658311</v>
       </c>
@@ -6299,7 +6298,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>14662611</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>14679871</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>14754308</v>
       </c>
@@ -6419,7 +6418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>14754423</v>
       </c>
@@ -6460,7 +6459,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>14755377</v>
       </c>
@@ -6501,7 +6500,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>14755551</v>
       </c>
@@ -6545,7 +6544,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>14755670</v>
       </c>
@@ -6589,7 +6588,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>14755852</v>
       </c>
@@ -6633,7 +6632,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>14756170</v>
       </c>
@@ -6674,7 +6673,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>14756343</v>
       </c>
@@ -6715,7 +6714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>14756916</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>14757031</v>
       </c>
@@ -6797,7 +6796,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>14757249</v>
       </c>
@@ -6841,7 +6840,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>14780346</v>
       </c>
@@ -6885,7 +6884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>14801617</v>
       </c>
@@ -6929,7 +6928,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>14837136</v>
       </c>
@@ -6973,7 +6972,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>14838346</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>14842341</v>
       </c>
@@ -7061,7 +7060,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>14842382</v>
       </c>
@@ -7105,7 +7104,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>14842445</v>
       </c>
@@ -7149,7 +7148,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>14851613</v>
       </c>
@@ -7193,7 +7192,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>14852581</v>
       </c>
@@ -7237,7 +7236,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>14852615</v>
       </c>
@@ -7281,7 +7280,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>14876575</v>
       </c>
@@ -7325,7 +7324,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>14876584</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>14876594</v>
       </c>
@@ -7413,7 +7412,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>14903409</v>
       </c>
@@ -7457,7 +7456,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>14913528</v>
       </c>
@@ -7501,7 +7500,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>14913543</v>
       </c>
@@ -7545,7 +7544,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>14913576</v>
       </c>
@@ -7592,7 +7591,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>14913615</v>
       </c>
@@ -7639,7 +7638,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>14951606</v>
       </c>
@@ -7683,7 +7682,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>14952039</v>
       </c>
@@ -7727,7 +7726,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>14953337</v>
       </c>
@@ -7768,7 +7767,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>14953442</v>
       </c>
@@ -7812,7 +7811,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>14953749</v>
       </c>
@@ -7856,7 +7855,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>14954824</v>
       </c>
@@ -7900,7 +7899,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>14954945</v>
       </c>
@@ -7944,7 +7943,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>14955065</v>
       </c>
@@ -7988,7 +7987,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>14955855</v>
       </c>
@@ -8032,7 +8031,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>14955882</v>
       </c>
@@ -8076,7 +8075,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>14956435</v>
       </c>
@@ -8120,7 +8119,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>14956707</v>
       </c>
@@ -8164,7 +8163,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>14957029</v>
       </c>
@@ -8208,7 +8207,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>14957950</v>
       </c>
@@ -8252,7 +8251,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>14960611</v>
       </c>
@@ -8296,7 +8295,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>14960769</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>14960875</v>
       </c>
@@ -8384,7 +8383,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>14961131</v>
       </c>
@@ -8428,7 +8427,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>14961380</v>
       </c>
@@ -8472,7 +8471,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>14961547</v>
       </c>
@@ -8516,7 +8515,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>14961738</v>
       </c>
@@ -8560,7 +8559,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>14962063</v>
       </c>
@@ -8604,7 +8603,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>14962251</v>
       </c>
@@ -8648,7 +8647,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>14962601</v>
       </c>
@@ -8692,7 +8691,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>14962883</v>
       </c>
@@ -8736,7 +8735,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>14964059</v>
       </c>
@@ -8780,7 +8779,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>14964141</v>
       </c>
@@ -8824,7 +8823,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>14964153</v>
       </c>
@@ -8868,7 +8867,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>14964681</v>
       </c>
@@ -8912,7 +8911,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>14964771</v>
       </c>
@@ -8956,7 +8955,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>14964871</v>
       </c>
@@ -9000,7 +8999,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>14965136</v>
       </c>
@@ -9044,7 +9043,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>14965357</v>
       </c>
@@ -9088,7 +9087,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>14965533</v>
       </c>
@@ -9132,7 +9131,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>14965687</v>
       </c>
@@ -9176,7 +9175,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>14965763</v>
       </c>
@@ -9220,7 +9219,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>14965898</v>
       </c>
@@ -9264,7 +9263,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>14965996</v>
       </c>
@@ -9308,7 +9307,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>14966154</v>
       </c>
@@ -9352,7 +9351,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>14966360</v>
       </c>
@@ -9396,7 +9395,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>14966616</v>
       </c>
@@ -9440,7 +9439,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>14966791</v>
       </c>
@@ -9484,7 +9483,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>14967024</v>
       </c>
@@ -9528,7 +9527,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>14967296</v>
       </c>
@@ -9572,7 +9571,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>14967616</v>
       </c>
@@ -9616,7 +9615,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>14967901</v>
       </c>
@@ -9660,7 +9659,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>14968154</v>
       </c>
@@ -9704,7 +9703,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>14968394</v>
       </c>
@@ -9748,7 +9747,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>14970182</v>
       </c>
@@ -9792,7 +9791,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>14989869</v>
       </c>
@@ -9836,7 +9835,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>14990074</v>
       </c>
@@ -9880,7 +9879,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>14990175</v>
       </c>
@@ -9924,7 +9923,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>14990576</v>
       </c>
@@ -9968,7 +9967,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>14990956</v>
       </c>
@@ -10015,7 +10014,7 @@
         <v>43312.443101851852</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>14991581</v>
       </c>
@@ -10059,7 +10058,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>14991667</v>
       </c>
@@ -10103,7 +10102,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>14992006</v>
       </c>
@@ -10147,7 +10146,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>14992066</v>
       </c>
@@ -10194,7 +10193,7 @@
         <v>43312.467939814815</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>15055138</v>
       </c>
@@ -10235,7 +10234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>15129462</v>
       </c>
@@ -10279,7 +10278,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>15129468</v>
       </c>
@@ -10323,7 +10322,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>15154990</v>
       </c>
@@ -10367,7 +10366,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>15162160</v>
       </c>
@@ -10411,7 +10410,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>15162168</v>
       </c>
@@ -10455,7 +10454,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>15162175</v>
       </c>
@@ -10499,7 +10498,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>15162399</v>
       </c>
@@ -10543,7 +10542,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>15162410</v>
       </c>
@@ -10587,7 +10586,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>15178303</v>
       </c>
@@ -10634,7 +10633,7 @@
         <v>43299.666666666664</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>15178453</v>
       </c>
@@ -10678,7 +10677,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>15178821</v>
       </c>
@@ -10725,7 +10724,7 @@
         <v>43299.694444444445</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>15178962</v>
       </c>
@@ -10769,7 +10768,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>15182383</v>
       </c>
@@ -10798,7 +10797,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>15182574</v>
       </c>
@@ -10827,7 +10826,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>15182638</v>
       </c>
@@ -10856,7 +10855,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>15182735</v>
       </c>
@@ -10885,7 +10884,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>15184056</v>
       </c>
@@ -10914,7 +10913,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>15191795</v>
       </c>
@@ -10958,7 +10957,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>15191800</v>
       </c>
@@ -11002,7 +11001,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>15204245</v>
       </c>
@@ -11043,7 +11042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>15204283</v>
       </c>
@@ -11084,7 +11083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>15204336</v>
       </c>
@@ -11125,7 +11124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>15204381</v>
       </c>
@@ -11163,7 +11162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>15204438</v>
       </c>
@@ -11207,7 +11206,7 @@
         <v>43307.427083333336</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>15206038</v>
       </c>
@@ -11251,7 +11250,7 @@
         <v>43307.427083333336</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>15206084</v>
       </c>
@@ -11292,7 +11291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>15263735</v>
       </c>
@@ -11336,7 +11335,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>15265404</v>
       </c>
@@ -11377,7 +11376,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>15265433</v>
       </c>
@@ -11421,7 +11420,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>15266287</v>
       </c>
@@ -11462,7 +11461,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>15275173</v>
       </c>
@@ -11503,7 +11502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>15275195</v>
       </c>
@@ -11544,7 +11543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>15275211</v>
       </c>
@@ -11585,7 +11584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>15275236</v>
       </c>
@@ -11626,7 +11625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>15328669</v>
       </c>
@@ -11670,7 +11669,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>15332546</v>
       </c>
@@ -11714,7 +11713,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>15334552</v>
       </c>
@@ -11758,7 +11757,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>15368823</v>
       </c>
@@ -11790,7 +11789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>15393294</v>
       </c>
@@ -11834,7 +11833,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>15393934</v>
       </c>
@@ -11878,7 +11877,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>15395747</v>
       </c>
@@ -11922,7 +11921,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>15395787</v>
       </c>
@@ -11966,7 +11965,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>15398996</v>
       </c>
@@ -12007,7 +12006,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>15399699</v>
       </c>
@@ -12051,7 +12050,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>15419259</v>
       </c>
@@ -12095,7 +12094,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>15419270</v>
       </c>
@@ -12136,7 +12135,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>15419277</v>
       </c>
@@ -12177,7 +12176,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>15419283</v>
       </c>
@@ -12221,7 +12220,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>15421432</v>
       </c>
@@ -12265,7 +12264,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>15421771</v>
       </c>
@@ -12309,7 +12308,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>15422138</v>
       </c>
@@ -12353,7 +12352,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>15422383</v>
       </c>
@@ -12397,7 +12396,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>15422493</v>
       </c>
@@ -12441,7 +12440,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>15422790</v>
       </c>
@@ -12485,7 +12484,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>15423055</v>
       </c>
@@ -12529,7 +12528,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>15423113</v>
       </c>
@@ -12573,7 +12572,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>15423211</v>
       </c>
@@ -12617,7 +12616,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>15423531</v>
       </c>
@@ -12661,7 +12660,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>15423616</v>
       </c>
@@ -12705,7 +12704,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>15462118</v>
       </c>
@@ -12755,7 +12754,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>15462176</v>
       </c>
@@ -12799,7 +12798,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>15462213</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>15462332</v>
       </c>
@@ -12887,7 +12886,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>15462404</v>
       </c>
@@ -12931,7 +12930,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>15462493</v>
       </c>
@@ -12975,7 +12974,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>15462539</v>
       </c>
@@ -13019,7 +13018,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>15462928</v>
       </c>
@@ -13063,7 +13062,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>15463002</v>
       </c>
@@ -13107,7 +13106,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>15463061</v>
       </c>
@@ -13151,7 +13150,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>15463109</v>
       </c>
@@ -13195,7 +13194,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>15518053</v>
       </c>
@@ -13245,7 +13244,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>15591650</v>
       </c>
@@ -13289,7 +13288,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>15591669</v>
       </c>
@@ -13333,7 +13332,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>15591686</v>
       </c>
@@ -13377,7 +13376,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>15627995</v>
       </c>
@@ -13421,7 +13420,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>15649639</v>
       </c>
@@ -13465,7 +13464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>15652459</v>
       </c>
@@ -13509,7 +13508,7 @@
         <v>43322.649305555555</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>15697962</v>
       </c>
@@ -13550,7 +13549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>15698041</v>
       </c>
@@ -13591,7 +13590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>15698070</v>
       </c>
@@ -13632,7 +13631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>15698097</v>
       </c>
@@ -13673,7 +13672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>15735906</v>
       </c>
@@ -13717,7 +13716,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>15737881</v>
       </c>
@@ -13761,7 +13760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>15769495</v>
       </c>
@@ -13802,7 +13801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>15847636</v>
       </c>
@@ -13843,7 +13842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>15847690</v>
       </c>
@@ -13881,7 +13880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>15847946</v>
       </c>
@@ -13925,7 +13924,7 @@
         <v>43335.458333333336</v>
       </c>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>15848069</v>
       </c>
@@ -13969,7 +13968,7 @@
         <v>43335.463194444441</v>
       </c>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>15864085</v>
       </c>
@@ -14013,7 +14012,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>15878216</v>
       </c>
@@ -14054,7 +14053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>15878666</v>
       </c>
@@ -14098,7 +14097,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>15881196</v>
       </c>
@@ -14136,7 +14135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>15881239</v>
       </c>
@@ -14180,7 +14179,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>15892302</v>
       </c>
@@ -14224,7 +14223,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>15903786</v>
       </c>
@@ -14268,7 +14267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>15913747</v>
       </c>
@@ -14282,7 +14281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>15915741</v>
       </c>
@@ -14326,7 +14325,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>15916211</v>
       </c>
@@ -14376,7 +14375,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>15916564</v>
       </c>
@@ -14426,7 +14425,7 @@
         <v>43333.333333333336</v>
       </c>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>15924898</v>
       </c>
@@ -14470,7 +14469,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>15925121</v>
       </c>
@@ -14514,7 +14513,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>15925428</v>
       </c>
@@ -14564,7 +14563,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>15925520</v>
       </c>
@@ -14614,7 +14613,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>15925587</v>
       </c>
@@ -14658,7 +14657,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>15926086</v>
       </c>
@@ -14702,7 +14701,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>15927247</v>
       </c>
@@ -14746,7 +14745,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>15927288</v>
       </c>
@@ -14790,7 +14789,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>15963803</v>
       </c>
@@ -14834,7 +14833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>15964648</v>
       </c>
@@ -14878,7 +14877,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>15978616</v>
       </c>
@@ -14922,7 +14921,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>15979438</v>
       </c>
@@ -14966,7 +14965,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>15980401</v>
       </c>
@@ -15010,7 +15009,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>15981482</v>
       </c>
@@ -15051,7 +15050,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>15982249</v>
       </c>
@@ -15089,7 +15088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>15982915</v>
       </c>
@@ -15133,7 +15132,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>15983560</v>
       </c>
@@ -15177,7 +15176,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>15986829</v>
       </c>
@@ -15221,7 +15220,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>15987614</v>
       </c>
@@ -15265,7 +15264,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>15987712</v>
       </c>
@@ -15309,7 +15308,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>15988312</v>
       </c>
@@ -15353,7 +15352,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>16012945</v>
       </c>
@@ -15397,7 +15396,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>16013634</v>
       </c>
@@ -15441,7 +15440,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>16053103</v>
       </c>
@@ -15485,7 +15484,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>16054624</v>
       </c>
@@ -15529,7 +15528,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>16057779</v>
       </c>
@@ -15573,7 +15572,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>16148657</v>
       </c>
@@ -15617,7 +15616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>16183159</v>
       </c>
@@ -15661,7 +15660,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>16219384</v>
       </c>
@@ -15705,7 +15704,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>16219451</v>
       </c>
@@ -15749,7 +15748,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>16219459</v>
       </c>
@@ -15793,7 +15792,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>16237856</v>
       </c>
@@ -15837,7 +15836,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>16240455</v>
       </c>
@@ -15881,7 +15880,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>16241407</v>
       </c>
@@ -15925,7 +15924,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>16263375</v>
       </c>
@@ -15966,7 +15965,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>16264742</v>
       </c>
@@ -16007,7 +16006,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>16285267</v>
       </c>
@@ -16051,7 +16050,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>16335937</v>
       </c>
@@ -16095,7 +16094,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>16336081</v>
       </c>
@@ -16139,7 +16138,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>16371170</v>
       </c>
@@ -16183,7 +16182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>16373515</v>
       </c>
@@ -16227,7 +16226,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>16508172</v>
       </c>
@@ -16271,7 +16270,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>16539231</v>
       </c>
@@ -16315,7 +16314,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>16539287</v>
       </c>
@@ -16359,7 +16358,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>16554941</v>
       </c>
@@ -16403,7 +16402,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>16555270</v>
       </c>
@@ -16447,7 +16446,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>16555473</v>
       </c>
@@ -16491,7 +16490,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>16555876</v>
       </c>
@@ -16535,7 +16534,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>16556207</v>
       </c>
@@ -16579,7 +16578,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>16613266</v>
       </c>
@@ -16620,7 +16619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>16640951</v>
       </c>
@@ -16664,7 +16663,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>16669884</v>
       </c>
@@ -16708,7 +16707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>16672653</v>
       </c>
@@ -16752,7 +16751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>16730239</v>
       </c>
@@ -16790,7 +16789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>16730385</v>
       </c>
@@ -16834,7 +16833,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>16730647</v>
       </c>
@@ -16872,7 +16871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>16731332</v>
       </c>
@@ -16910,7 +16909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>16731607</v>
       </c>
@@ -16954,7 +16953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>16731630</v>
       </c>
@@ -16998,7 +16997,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>16731997</v>
       </c>
@@ -17042,7 +17041,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>16735025</v>
       </c>
@@ -17086,7 +17085,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>16735293</v>
       </c>
@@ -17130,7 +17129,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>16735337</v>
       </c>
@@ -17174,7 +17173,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>16735400</v>
       </c>
@@ -17218,7 +17217,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>16735514</v>
       </c>
@@ -17262,7 +17261,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>16756371</v>
       </c>
@@ -17306,7 +17305,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>16756517</v>
       </c>
@@ -17350,7 +17349,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>16756927</v>
       </c>
@@ -17394,7 +17393,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>16757207</v>
       </c>
@@ -17438,7 +17437,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>16757508</v>
       </c>
@@ -17482,7 +17481,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>16757699</v>
       </c>
@@ -17526,7 +17525,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>16758179</v>
       </c>
@@ -17570,7 +17569,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>16758583</v>
       </c>
@@ -17614,7 +17613,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>16758943</v>
       </c>
@@ -17658,7 +17657,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>16759208</v>
       </c>
@@ -17702,7 +17701,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>16759509</v>
       </c>
@@ -17746,7 +17745,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>16759922</v>
       </c>
@@ -17790,7 +17789,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>16760418</v>
       </c>
@@ -17834,7 +17833,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="339" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>16761901</v>
       </c>
@@ -17878,7 +17877,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="340" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>16762060</v>
       </c>
@@ -17922,7 +17921,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>16762161</v>
       </c>
@@ -17966,7 +17965,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>16762364</v>
       </c>
@@ -18010,7 +18009,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>16762693</v>
       </c>
@@ -18054,7 +18053,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>16763180</v>
       </c>
@@ -18098,7 +18097,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>16763783</v>
       </c>
@@ -18142,7 +18141,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>16764001</v>
       </c>
@@ -18186,7 +18185,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>16764262</v>
       </c>
@@ -18230,7 +18229,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>16764468</v>
       </c>
@@ -18274,7 +18273,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>16764627</v>
       </c>
@@ -18318,7 +18317,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>16764760</v>
       </c>
@@ -18362,7 +18361,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>16765462</v>
       </c>
@@ -18412,16 +18411,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B163" sqref="B1:C163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>501</v>
       </c>
@@ -18432,7 +18431,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>504</v>
       </c>
@@ -18443,7 +18442,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>507</v>
       </c>
@@ -18454,7 +18453,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>510</v>
       </c>
@@ -18465,7 +18464,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>513</v>
       </c>
@@ -18476,7 +18475,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>516</v>
       </c>
@@ -18487,7 +18486,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>518</v>
       </c>
@@ -18498,7 +18497,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>521</v>
       </c>
@@ -18509,7 +18508,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>524</v>
       </c>
@@ -18520,7 +18519,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>527</v>
       </c>
@@ -18531,7 +18530,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>530</v>
       </c>
@@ -18542,7 +18541,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>533</v>
       </c>
@@ -18553,7 +18552,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>279</v>
       </c>
@@ -18564,7 +18563,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>537</v>
       </c>
@@ -18575,7 +18574,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>540</v>
       </c>
@@ -18586,7 +18585,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>543</v>
       </c>
@@ -18597,7 +18596,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>546</v>
       </c>
@@ -18608,7 +18607,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>549</v>
       </c>
@@ -18619,7 +18618,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>552</v>
       </c>
@@ -18630,7 +18629,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>553</v>
       </c>
@@ -18641,7 +18640,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>556</v>
       </c>
@@ -18652,7 +18651,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>559</v>
       </c>
@@ -18663,7 +18662,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>562</v>
       </c>
@@ -18674,7 +18673,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>564</v>
       </c>
@@ -18685,7 +18684,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>567</v>
       </c>
@@ -18696,7 +18695,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>570</v>
       </c>
@@ -18707,7 +18706,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>573</v>
       </c>
@@ -18718,7 +18717,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>576</v>
       </c>
@@ -18729,7 +18728,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>579</v>
       </c>
@@ -18740,7 +18739,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>582</v>
       </c>
@@ -18751,7 +18750,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>585</v>
       </c>
@@ -18762,7 +18761,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>586</v>
       </c>
@@ -18773,7 +18772,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>302</v>
       </c>
@@ -18784,7 +18783,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>591</v>
       </c>
@@ -18795,7 +18794,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>594</v>
       </c>
@@ -18806,7 +18805,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>123</v>
       </c>
@@ -18817,7 +18816,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>599</v>
       </c>
@@ -18828,7 +18827,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>602</v>
       </c>
@@ -18839,7 +18838,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>604</v>
       </c>
@@ -18850,7 +18849,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>607</v>
       </c>
@@ -18861,7 +18860,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>610</v>
       </c>
@@ -18872,7 +18871,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>610</v>
       </c>
@@ -18883,7 +18882,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>613</v>
       </c>
@@ -18894,7 +18893,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>616</v>
       </c>
@@ -18905,7 +18904,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>619</v>
       </c>
@@ -18916,7 +18915,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>622</v>
       </c>
@@ -18927,7 +18926,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>625</v>
       </c>
@@ -18938,7 +18937,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>628</v>
       </c>
@@ -18949,7 +18948,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>631</v>
       </c>
@@ -18960,7 +18959,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>634</v>
       </c>
@@ -18971,7 +18970,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>636</v>
       </c>
@@ -18982,7 +18981,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>638</v>
       </c>
@@ -18993,7 +18992,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>641</v>
       </c>
@@ -19004,7 +19003,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>644</v>
       </c>
@@ -19015,7 +19014,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>647</v>
       </c>
@@ -19026,7 +19025,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>650</v>
       </c>
@@ -19037,7 +19036,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>653</v>
       </c>
@@ -19048,7 +19047,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>656</v>
       </c>
@@ -19059,7 +19058,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>659</v>
       </c>
@@ -19070,7 +19069,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>662</v>
       </c>
@@ -19081,7 +19080,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>665</v>
       </c>
@@ -19092,7 +19091,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>667</v>
       </c>
@@ -19103,7 +19102,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>669</v>
       </c>
@@ -19114,7 +19113,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>672</v>
       </c>
@@ -19125,7 +19124,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>675</v>
       </c>
@@ -19136,7 +19135,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>678</v>
       </c>
@@ -19147,7 +19146,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>139</v>
       </c>
@@ -19158,7 +19157,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>682</v>
       </c>
@@ -19169,7 +19168,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>685</v>
       </c>
@@ -19180,7 +19179,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>688</v>
       </c>
@@ -19191,7 +19190,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>691</v>
       </c>
@@ -19202,7 +19201,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>694</v>
       </c>
@@ -19213,7 +19212,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>697</v>
       </c>
@@ -19224,7 +19223,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>700</v>
       </c>
@@ -19235,7 +19234,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>703</v>
       </c>
@@ -19246,7 +19245,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>706</v>
       </c>
@@ -19257,7 +19256,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>709</v>
       </c>
@@ -19268,7 +19267,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>712</v>
       </c>
@@ -19279,7 +19278,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>713</v>
       </c>
@@ -19290,7 +19289,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>716</v>
       </c>
@@ -19301,7 +19300,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>719</v>
       </c>
@@ -19312,7 +19311,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>722</v>
       </c>
@@ -19323,7 +19322,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>725</v>
       </c>
@@ -19334,7 +19333,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>727</v>
       </c>
@@ -19345,7 +19344,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>730</v>
       </c>
@@ -19356,7 +19355,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>733</v>
       </c>
@@ -19367,7 +19366,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
         <v>736</v>
       </c>
@@ -19378,7 +19377,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>739</v>
       </c>
@@ -19389,7 +19388,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
         <v>742</v>
       </c>
@@ -19400,7 +19399,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
         <v>745</v>
       </c>
@@ -19411,7 +19410,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
         <v>747</v>
       </c>
@@ -19422,7 +19421,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
         <v>749</v>
       </c>
@@ -19433,7 +19432,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
         <v>750</v>
       </c>
@@ -19444,7 +19443,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
         <v>752</v>
       </c>
@@ -19455,7 +19454,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
         <v>755</v>
       </c>
@@ -19466,7 +19465,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
         <v>739</v>
       </c>
@@ -19477,7 +19476,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
         <v>760</v>
       </c>
@@ -19488,7 +19487,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
         <v>116</v>
       </c>
@@ -19499,7 +19498,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
         <v>747</v>
       </c>
@@ -19510,7 +19509,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>764</v>
       </c>
@@ -19521,7 +19520,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
         <v>767</v>
       </c>
@@ -19532,7 +19531,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
         <v>770</v>
       </c>
@@ -19543,7 +19542,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
         <v>773</v>
       </c>
@@ -19554,7 +19553,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
         <v>776</v>
       </c>
@@ -19565,7 +19564,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
         <v>778</v>
       </c>
@@ -19576,7 +19575,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
         <v>780</v>
       </c>
@@ -19587,7 +19586,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
         <v>783</v>
       </c>
@@ -19598,7 +19597,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
         <v>784</v>
       </c>
@@ -19609,7 +19608,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>786</v>
       </c>
@@ -19620,7 +19619,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>14</v>
       </c>
@@ -19631,7 +19630,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
         <v>790</v>
       </c>
@@ -19642,7 +19641,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
         <v>792</v>
       </c>
@@ -19653,7 +19652,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>53</v>
       </c>
@@ -19664,7 +19663,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
         <v>84</v>
       </c>
@@ -19675,7 +19674,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
         <v>156</v>
       </c>
@@ -19686,7 +19685,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
         <v>800</v>
       </c>
@@ -19697,7 +19696,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>803</v>
       </c>
@@ -19708,7 +19707,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
         <v>149</v>
       </c>
@@ -19719,7 +19718,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
         <v>808</v>
       </c>
@@ -19730,7 +19729,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
         <v>810</v>
       </c>
@@ -19741,7 +19740,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
         <v>813</v>
       </c>
@@ -19752,7 +19751,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
         <v>816</v>
       </c>
@@ -19763,7 +19762,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
         <v>277</v>
       </c>
@@ -19774,7 +19773,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
         <v>820</v>
       </c>
@@ -19785,7 +19784,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
         <v>823</v>
       </c>
@@ -19796,7 +19795,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
         <v>826</v>
       </c>
@@ -19807,7 +19806,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
         <v>828</v>
       </c>
@@ -19818,7 +19817,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
         <v>168</v>
       </c>
@@ -19829,7 +19828,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
         <v>833</v>
       </c>
@@ -19840,7 +19839,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
         <v>836</v>
       </c>
@@ -19851,7 +19850,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
         <v>839</v>
       </c>
@@ -19862,7 +19861,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>842</v>
       </c>
@@ -19873,7 +19872,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>845</v>
       </c>
@@ -19884,7 +19883,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
         <v>848</v>
       </c>
@@ -19895,7 +19894,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
         <v>850</v>
       </c>
@@ -19906,7 +19905,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
         <v>853</v>
       </c>
@@ -19917,7 +19916,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>856</v>
       </c>
@@ -19928,7 +19927,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
         <v>859</v>
       </c>
@@ -19939,7 +19938,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>861</v>
       </c>
@@ -19950,7 +19949,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
         <v>862</v>
       </c>
@@ -19961,7 +19960,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
         <v>865</v>
       </c>
@@ -19972,7 +19971,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
         <v>867</v>
       </c>
@@ -19983,7 +19982,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
         <v>870</v>
       </c>
@@ -19994,7 +19993,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
         <v>873</v>
       </c>
@@ -20005,7 +20004,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
         <v>876</v>
       </c>
@@ -20016,7 +20015,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
         <v>879</v>
       </c>
@@ -20027,7 +20026,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
         <v>882</v>
       </c>
@@ -20038,7 +20037,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
         <v>885</v>
       </c>
@@ -20049,7 +20048,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="8" t="s">
         <v>888</v>
       </c>
@@ -20060,7 +20059,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>890</v>
       </c>
@@ -20071,7 +20070,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
         <v>893</v>
       </c>
@@ -20082,7 +20081,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
         <v>896</v>
       </c>
@@ -20093,7 +20092,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
         <v>75</v>
       </c>
@@ -20104,7 +20103,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="8" t="s">
         <v>23</v>
       </c>
@@ -20115,7 +20114,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="8" t="s">
         <v>903</v>
       </c>
@@ -20126,7 +20125,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="8" t="s">
         <v>906</v>
       </c>
@@ -20137,7 +20136,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="8" t="s">
         <v>909</v>
       </c>
@@ -20148,7 +20147,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>288</v>
       </c>
@@ -20159,7 +20158,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>911</v>
       </c>
@@ -20170,7 +20169,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>75</v>
       </c>
@@ -20181,7 +20180,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
         <v>915</v>
       </c>
@@ -20192,7 +20191,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
         <v>918</v>
       </c>
@@ -20203,7 +20202,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
         <v>921</v>
       </c>

</xml_diff>